<commit_message>
Clean CAT data but waiting on ATM history
</commit_message>
<xml_diff>
--- a/data/raw/CAT_Options_Data.xlsx
+++ b/data/raw/CAT_Options_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/david_crowe_ucdconnect_ie/Documents/Masters/FIN42020 - Derivative Securities/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/david_crowe_ucdconnect_ie/Documents/Masters/FIN42020 - Derivative Securities/Project/FIN42020-Derivative-Securities-Project/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{1FD50B2D-D1A4-41A4-ADFD-D06D56F95791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C63DE39-266A-4164-B8FE-7C634B9CF545}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{1FD50B2D-D1A4-41A4-ADFD-D06D56F95791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A28B259D-590E-4D92-BFA9-C85FCC48993F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calls" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Price" sheetId="3" r:id="rId3"/>
     <sheet name="USGG1M" sheetId="4" r:id="rId4"/>
     <sheet name="ATM" sheetId="5" r:id="rId5"/>
+    <sheet name="Metadata" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
-  <si>
-    <t>Calls</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>Strike</t>
   </si>
@@ -63,9 +61,6 @@
     <t>Volm</t>
   </si>
   <si>
-    <t>17-Oct-25 (28d); CSize 100</t>
-  </si>
-  <si>
     <t>CAT 10/17/25 C340</t>
   </si>
   <si>
@@ -216,33 +211,6 @@
     <t>CAT 10/17/25 P600</t>
   </si>
   <si>
-    <t>Puts</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>CAT US Equity</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>Period</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -252,23 +220,227 @@
     <t>PX_BID</t>
   </si>
   <si>
-    <t>USGG1M Index</t>
-  </si>
-  <si>
-    <t>CHG_PCT_1D</t>
-  </si>
-  <si>
     <t>PX_VOLUME</t>
   </si>
   <si>
     <t>IVOL_MONEYNESS</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is a standard </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>option chain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>one single date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (17 October 2025).</t>
+    </r>
+  </si>
+  <si>
+    <t>The same</t>
+  </si>
+  <si>
+    <t>This is the only problem.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It has </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>one row</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from the option chain:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> an ATM time series.</t>
+    </r>
+  </si>
+  <si>
+    <t>It is just one observation for one date.</t>
+  </si>
+  <si>
+    <t>From the bottom of the Price sheet:</t>
+  </si>
+  <si>
+    <t>Trade date = 2025-08-19</t>
+  </si>
+  <si>
+    <t>Underlying price (PX_LAST) = 416.09</t>
+  </si>
+  <si>
+    <t>This is the day you enter the option position for the delta hedge.</t>
+  </si>
+  <si>
+    <t>This is the ONLY correct date to determine the ATM strike.</t>
+  </si>
+  <si>
+    <t>Correct ATM strike selection</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trade-date underlying price = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>416.09</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Closest strike to 416.09 is 420.</t>
+  </si>
+  <si>
+    <t>So the ATM strike is:</t>
+  </si>
+  <si>
+    <t>CAT 10/17/25 C420 (or P420, but call is standard)</t>
+  </si>
+  <si>
+    <t>This is your ATM option.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You need the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>daily price</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of: CAT 10/17/25 C420 2025-08-19 → 2025-10-17</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Calls Sheets</t>
+  </si>
+  <si>
+    <t>2. Puts Sheet</t>
+  </si>
+  <si>
+    <t>3. Price Sheet</t>
+  </si>
+  <si>
+    <t>4. USGG1M sheet</t>
+  </si>
+  <si>
+    <t>This is the stock price history.</t>
+  </si>
+  <si>
+    <t>Rate data</t>
+  </si>
+  <si>
+    <t>5. ATM sheet</t>
+  </si>
+  <si>
+    <t>For the delta hedging simulation, the project requires:“Daily prices of the same ATM option from the trade date up to expiration.”</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +577,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -755,8 +935,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1103,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView zoomScale="88" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1122,729 +1302,705 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>340</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>126.800003051758</v>
+      </c>
+      <c r="D2">
+        <v>128.69999694824199</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>54.544857025146499</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>350</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>116.849990844727</v>
+      </c>
+      <c r="D3">
+        <v>118.800003051758</v>
+      </c>
+      <c r="E3">
+        <v>117.220001220703</v>
+      </c>
+      <c r="F3">
+        <v>50.927101135253899</v>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>126.800003051758</v>
+        <v>106.10000610351599</v>
       </c>
       <c r="D4">
-        <v>128.69999694824199</v>
+        <v>108.599990844727</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>108.050003051758</v>
       </c>
       <c r="F4">
-        <v>54.544857025146499</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>116.849990844727</v>
+        <v>97.099990844726605</v>
       </c>
       <c r="D5">
-        <v>118.800003051758</v>
+        <v>98.899993896484403</v>
       </c>
       <c r="E5">
-        <v>117.220001220703</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>50.927101135253899</v>
+        <v>43.885978698730497</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>106.10000610351599</v>
+        <v>86.899993896484403</v>
       </c>
       <c r="D6">
-        <v>108.599990844727</v>
+        <v>89.050003051757798</v>
       </c>
       <c r="E6">
-        <v>108.050003051758</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>38.892742156982401</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>97.099990844726605</v>
+        <v>77.699996948242202</v>
       </c>
       <c r="D7">
-        <v>98.899993896484403</v>
+        <v>78.800003051757798</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>76.669998168945298</v>
       </c>
       <c r="F7">
-        <v>43.885978698730497</v>
+        <v>37.259841918945298</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>86.899993896484403</v>
+        <v>66.800003051757798</v>
       </c>
       <c r="D8">
-        <v>89.050003051757798</v>
+        <v>70.099990844726605</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>68.800003051757798</v>
       </c>
       <c r="F8">
-        <v>38.892742156982401</v>
+        <v>34.281211853027301</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>77.699996948242202</v>
+        <v>57.5</v>
       </c>
       <c r="D9">
-        <v>78.800003051757798</v>
+        <v>59.199996948242202</v>
       </c>
       <c r="E9">
-        <v>76.669998168945298</v>
+        <v>58.550003051757798</v>
       </c>
       <c r="F9">
-        <v>37.259841918945298</v>
+        <v>28.890645980835</v>
       </c>
       <c r="G9">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10">
-        <v>66.800003051757798</v>
+        <v>48.099990844726598</v>
       </c>
       <c r="D10">
-        <v>70.099990844726605</v>
+        <v>50.75</v>
       </c>
       <c r="E10">
-        <v>68.800003051757798</v>
+        <v>48.900009155273402</v>
       </c>
       <c r="F10">
-        <v>34.281211853027301</v>
+        <v>30.160873413085898</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>410</v>
+        <v>430</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>57.5</v>
+        <v>40.149993896484403</v>
       </c>
       <c r="D11">
-        <v>59.199996948242202</v>
+        <v>40.649993896484403</v>
       </c>
       <c r="E11">
-        <v>58.550003051757798</v>
+        <v>41.400009155273402</v>
       </c>
       <c r="F11">
-        <v>28.890645980835</v>
+        <v>28.661460876464801</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>420</v>
+        <v>440</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12">
-        <v>48.099990844726598</v>
+        <v>31.6499938964844</v>
       </c>
       <c r="D12">
-        <v>50.75</v>
+        <v>32.199996948242202</v>
       </c>
       <c r="E12">
-        <v>48.900009155273402</v>
+        <v>31.139999389648398</v>
       </c>
       <c r="F12">
-        <v>30.160873413085898</v>
+        <v>27.4340915679932</v>
       </c>
       <c r="G12">
-        <v>570</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>430</v>
+        <v>450</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13">
-        <v>40.149993896484403</v>
+        <v>23.8999938964844</v>
       </c>
       <c r="D13">
-        <v>40.649993896484403</v>
+        <v>24.349990844726602</v>
       </c>
       <c r="E13">
-        <v>41.400009155273402</v>
+        <v>24.449996948242202</v>
       </c>
       <c r="F13">
-        <v>28.661460876464801</v>
+        <v>26.210058212280298</v>
       </c>
       <c r="G13">
-        <v>45</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>440</v>
+        <v>460</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14">
-        <v>31.6499938964844</v>
+        <v>17.25</v>
       </c>
       <c r="D14">
-        <v>32.199996948242202</v>
+        <v>18</v>
       </c>
       <c r="E14">
-        <v>31.139999389648398</v>
+        <v>18.050003051757798</v>
       </c>
       <c r="F14">
-        <v>27.4340915679932</v>
+        <v>25.8072319030762</v>
       </c>
       <c r="G14">
-        <v>82</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15">
-        <v>23.8999938964844</v>
+        <v>11.8500003814697</v>
       </c>
       <c r="D15">
-        <v>24.349990844726602</v>
+        <v>12.1000003814697</v>
       </c>
       <c r="E15">
-        <v>24.449996948242202</v>
+        <v>12.1000003814697</v>
       </c>
       <c r="F15">
-        <v>26.210058212280298</v>
+        <v>24.875341415405298</v>
       </c>
       <c r="G15">
-        <v>180</v>
+        <v>836</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C16">
-        <v>17.25</v>
+        <v>7.6999998092651403</v>
       </c>
       <c r="D16">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E16">
-        <v>18.050003051757798</v>
+        <v>8.0600004196166992</v>
       </c>
       <c r="F16">
-        <v>25.8072319030762</v>
+        <v>24.597297668456999</v>
       </c>
       <c r="G16">
-        <v>170</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>470</v>
+        <v>490</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C17">
-        <v>11.8500003814697</v>
+        <v>4.6999998092651403</v>
       </c>
       <c r="D17">
-        <v>12.1000003814697</v>
+        <v>4.9499998092651403</v>
       </c>
       <c r="E17">
-        <v>12.1000003814697</v>
+        <v>4.9000005722045898</v>
       </c>
       <c r="F17">
-        <v>24.875341415405298</v>
+        <v>24.270544052123999</v>
       </c>
       <c r="G17">
-        <v>836</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>480</v>
+        <v>500</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C18">
-        <v>7.6999998092651403</v>
+        <v>2.8000001907348602</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>2.9899997711181601</v>
       </c>
       <c r="E18">
-        <v>8.0600004196166992</v>
+        <v>3.1000003814697301</v>
       </c>
       <c r="F18">
-        <v>24.597297668456999</v>
+        <v>24.3177890777588</v>
       </c>
       <c r="G18">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>490</v>
+        <v>510</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19">
-        <v>4.6999998092651403</v>
+        <v>1.5599994659423799</v>
       </c>
       <c r="D19">
-        <v>4.9499998092651403</v>
+        <v>1.75</v>
       </c>
       <c r="E19">
-        <v>4.9000005722045898</v>
+        <v>1.71000003814697</v>
       </c>
       <c r="F19">
-        <v>24.270544052123999</v>
+        <v>24.359022140502901</v>
       </c>
       <c r="G19">
-        <v>179</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>500</v>
+        <v>520</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20">
-        <v>2.8000001907348602</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>2.9899997711181601</v>
+        <v>1.09000015258789</v>
       </c>
       <c r="E20">
-        <v>3.1000003814697301</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>24.3177890777588</v>
+        <v>25.456571578979499</v>
       </c>
       <c r="G20">
-        <v>126</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>510</v>
+        <v>530</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21">
-        <v>1.5599994659423799</v>
+        <v>2.9999997466802601E-2</v>
       </c>
       <c r="D21">
-        <v>1.75</v>
+        <v>1.4899997711181601</v>
       </c>
       <c r="E21">
-        <v>1.71000003814697</v>
+        <v>0.60000002384185802</v>
       </c>
       <c r="F21">
-        <v>24.359022140502901</v>
+        <v>26.7674045562744</v>
       </c>
       <c r="G21">
-        <v>25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>520</v>
+        <v>540</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>5.0000000745058101E-2</v>
       </c>
       <c r="D22">
-        <v>1.09000015258789</v>
+        <v>0.62000000476837203</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.37000000476837203</v>
       </c>
       <c r="F22">
-        <v>25.456571578979499</v>
+        <v>25.866327285766602</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23">
-        <v>2.9999997466802601E-2</v>
+        <v>0.150000035762787</v>
       </c>
       <c r="D23">
-        <v>1.4899997711181601</v>
+        <v>0.730000019073486</v>
       </c>
       <c r="E23">
-        <v>0.60000002384185802</v>
+        <v>0.37000000476837203</v>
       </c>
       <c r="F23">
-        <v>26.7674045562744</v>
+        <v>29.860620498657202</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24">
-        <v>5.0000000745058101E-2</v>
+        <v>9.9999979138374294E-3</v>
       </c>
       <c r="D24">
-        <v>0.62000000476837203</v>
+        <v>0.5</v>
       </c>
       <c r="E24">
-        <v>0.37000000476837203</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>25.866327285766602</v>
+        <v>29.9681587219238</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>550</v>
+        <v>580</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25">
-        <v>0.150000035762787</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0.730000019073486</v>
+        <v>0.19999998807907099</v>
       </c>
       <c r="E25">
-        <v>0.37000000476837203</v>
+        <v>0.10000002384185799</v>
       </c>
       <c r="F25">
-        <v>29.860620498657202</v>
+        <v>33.7088623046875</v>
       </c>
       <c r="G25">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>560</v>
+        <v>600</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26">
-        <v>9.9999979138374294E-3</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0.5</v>
+        <v>0.28000003099441501</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>7.9999983310699505E-2</v>
       </c>
       <c r="F26">
-        <v>29.9681587219238</v>
+        <v>39.942710876464801</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>580</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0.19999998807907099</v>
-      </c>
-      <c r="E27">
-        <v>0.10000002384185799</v>
-      </c>
-      <c r="F27">
-        <v>33.7088623046875</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>600</v>
-      </c>
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0.28000003099441501</v>
-      </c>
-      <c r="E28">
-        <v>7.9999983310699505E-2</v>
-      </c>
-      <c r="F28">
-        <v>39.942710876464801</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A83:G83"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A41:G41"/>
+  <mergeCells count="10">
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A69:G69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1852,10 +2008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EEAAB3-C1BD-4CDB-9A53-F7DA5D360A02}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1868,96 +2024,137 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>340</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>5.0000000745058101E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.259999990463257</v>
+      </c>
+      <c r="E2">
+        <v>0.150000035762787</v>
+      </c>
+      <c r="F2">
+        <v>47.592529296875</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>350</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.519999980926514</v>
+      </c>
+      <c r="E3">
+        <v>0.240000009536743</v>
+      </c>
+      <c r="F3">
+        <v>51.844081878662102</v>
+      </c>
+      <c r="G3">
         <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>5.0000000745058101E-2</v>
+        <v>0.10000002384185799</v>
       </c>
       <c r="D4">
-        <v>0.259999990463257</v>
+        <v>0.55000001192092896</v>
       </c>
       <c r="E4">
-        <v>0.150000035762787</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>47.592529296875</v>
+        <v>44.148311614990199</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>0.21999996900558499</v>
+      </c>
+      <c r="D5">
+        <v>0.38999998569488498</v>
+      </c>
+      <c r="E5">
+        <v>0.230000019073486</v>
+      </c>
+      <c r="F5">
+        <v>39.720550537109403</v>
+      </c>
+      <c r="G5">
         <v>12</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0.519999980926514</v>
-      </c>
-      <c r="E5">
-        <v>0.240000009536743</v>
-      </c>
-      <c r="F5">
-        <v>51.844081878662102</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>360</v>
+        <v>380</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>0.10000002384185799</v>
+        <v>0.25</v>
       </c>
       <c r="D6">
-        <v>0.55000001192092896</v>
+        <v>0.490000009536743</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>44.148311614990199</v>
+        <v>36.851699829101598</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1965,275 +2162,275 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>0.21999996900558499</v>
+        <v>0.46000003814697299</v>
       </c>
       <c r="D7">
-        <v>0.38999998569488498</v>
+        <v>0.54000002145767201</v>
       </c>
       <c r="E7">
-        <v>0.230000019073486</v>
+        <v>0.58999997377395597</v>
       </c>
       <c r="F7">
-        <v>39.720550537109403</v>
+        <v>34.564407348632798</v>
       </c>
       <c r="G7">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>0.25</v>
+        <v>0.66000002622604403</v>
       </c>
       <c r="D8">
-        <v>0.490000009536743</v>
+        <v>0.82999998331069902</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.80000001192092896</v>
       </c>
       <c r="F8">
-        <v>36.851699829101598</v>
+        <v>32.8298530578613</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>0.46000003814697299</v>
+        <v>1.0299997329711901</v>
       </c>
       <c r="D9">
-        <v>0.54000002145767201</v>
+        <v>1.1499996185302701</v>
       </c>
       <c r="E9">
-        <v>0.58999997377395597</v>
+        <v>1.13000011444092</v>
       </c>
       <c r="F9">
-        <v>34.564407348632798</v>
+        <v>30.959781646728501</v>
       </c>
       <c r="G9">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>0.66000002622604403</v>
+        <v>1.36999988555908</v>
       </c>
       <c r="D10">
-        <v>0.82999998331069902</v>
+        <v>1.7799997329711901</v>
       </c>
       <c r="E10">
-        <v>0.80000001192092896</v>
+        <v>1.65999984741211</v>
       </c>
       <c r="F10">
-        <v>32.8298530578613</v>
+        <v>28.954750061035199</v>
       </c>
       <c r="G10">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>410</v>
+        <v>430</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11">
-        <v>1.0299997329711901</v>
+        <v>2.4499998092651398</v>
       </c>
       <c r="D11">
-        <v>1.1499996185302701</v>
+        <v>2.96000003814697</v>
       </c>
       <c r="E11">
-        <v>1.13000011444092</v>
+        <v>2.5699996948242201</v>
       </c>
       <c r="F11">
-        <v>30.959781646728501</v>
+        <v>28.402624130248999</v>
       </c>
       <c r="G11">
-        <v>30</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>420</v>
+        <v>440</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C12">
-        <v>1.36999988555908</v>
+        <v>3.9000005722045898</v>
       </c>
       <c r="D12">
-        <v>1.7799997329711901</v>
+        <v>4.1500005722045898</v>
       </c>
       <c r="E12">
-        <v>1.65999984741211</v>
+        <v>3.9899997711181601</v>
       </c>
       <c r="F12">
-        <v>28.954750061035199</v>
+        <v>26.742303848266602</v>
       </c>
       <c r="G12">
-        <v>44</v>
+        <v>978</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>430</v>
+        <v>450</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13">
-        <v>2.4499998092651398</v>
+        <v>6.0999994277954102</v>
       </c>
       <c r="D13">
-        <v>2.96000003814697</v>
+        <v>6.9499998092651403</v>
       </c>
       <c r="E13">
-        <v>2.5699996948242201</v>
+        <v>6.6800003051757804</v>
       </c>
       <c r="F13">
-        <v>28.402624130248999</v>
+        <v>26.347204208373999</v>
       </c>
       <c r="G13">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>440</v>
+        <v>460</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14">
-        <v>3.9000005722045898</v>
+        <v>9.3999996185302699</v>
       </c>
       <c r="D14">
-        <v>4.1500005722045898</v>
+        <v>9.6999998092651403</v>
       </c>
       <c r="E14">
-        <v>3.9899997711181601</v>
+        <v>9.5500001907348597</v>
       </c>
       <c r="F14">
-        <v>26.742303848266602</v>
+        <v>24.9950046539307</v>
       </c>
       <c r="G14">
-        <v>978</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15">
-        <v>6.0999994277954102</v>
+        <v>13.8999996185303</v>
       </c>
       <c r="D15">
-        <v>6.9499998092651403</v>
+        <v>14.25</v>
       </c>
       <c r="E15">
-        <v>6.6800003051757804</v>
+        <v>14.050000190734901</v>
       </c>
       <c r="F15">
-        <v>26.347204208373999</v>
+        <v>24.387588500976602</v>
       </c>
       <c r="G15">
-        <v>44</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C16">
-        <v>9.3999996185302699</v>
+        <v>19.849990844726602</v>
       </c>
       <c r="D16">
-        <v>9.6999998092651403</v>
+        <v>21.2999877929688</v>
       </c>
       <c r="E16">
-        <v>9.5500001907348597</v>
+        <v>22.25</v>
       </c>
       <c r="F16">
-        <v>24.9950046539307</v>
+        <v>25.2547092437744</v>
       </c>
       <c r="G16">
-        <v>174</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>470</v>
+        <v>490</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C17">
-        <v>13.8999996185303</v>
+        <v>26.8999938964844</v>
       </c>
       <c r="D17">
-        <v>14.25</v>
+        <v>28.5</v>
       </c>
       <c r="E17">
-        <v>14.050000190734901</v>
+        <v>28.800003051757798</v>
       </c>
       <c r="F17">
-        <v>24.387588500976602</v>
+        <v>25.195888519287099</v>
       </c>
       <c r="G17">
-        <v>79</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>480</v>
+        <v>500</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C18">
-        <v>19.849990844726602</v>
+        <v>35</v>
       </c>
       <c r="D18">
-        <v>21.2999877929688</v>
+        <v>35.75</v>
       </c>
       <c r="E18">
-        <v>22.25</v>
+        <v>34</v>
       </c>
       <c r="F18">
-        <v>25.2547092437744</v>
+        <v>23.849817276001001</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2241,68 +2438,68 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>490</v>
+        <v>510</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C19">
-        <v>26.8999938964844</v>
+        <v>43.449996948242202</v>
       </c>
       <c r="D19">
-        <v>28.5</v>
+        <v>45.350006103515597</v>
       </c>
       <c r="E19">
-        <v>28.800003051757798</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>25.195888519287099</v>
+        <v>24.080043792724599</v>
       </c>
       <c r="G19">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>500</v>
+        <v>520</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C20">
-        <v>35</v>
+        <v>52.400009155273402</v>
       </c>
       <c r="D20">
-        <v>35.75</v>
+        <v>55.199996948242202</v>
       </c>
       <c r="E20">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>23.849817276001001</v>
+        <v>21.775556564331101</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>510</v>
+        <v>530</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C21">
-        <v>43.449996948242202</v>
+        <v>62.399993896484403</v>
       </c>
       <c r="D21">
-        <v>45.350006103515597</v>
+        <v>65</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
-        <v>24.080043792724599</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2310,22 +2507,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>520</v>
+        <v>540</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C22">
-        <v>52.400009155273402</v>
+        <v>72.199996948242202</v>
       </c>
       <c r="D22">
-        <v>55.199996948242202</v>
+        <v>74.800003051757798</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
-        <v>21.775556564331101</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2333,16 +2530,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>530</v>
+        <v>550</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C23">
-        <v>62.399993896484403</v>
+        <v>82.550003051757798</v>
       </c>
       <c r="D23">
-        <v>65</v>
+        <v>84.5</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2356,16 +2553,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C24">
-        <v>72.199996948242202</v>
+        <v>92.5</v>
       </c>
       <c r="D24">
-        <v>74.800003051757798</v>
+        <v>94.800003051757798</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2379,39 +2576,39 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>550</v>
+        <v>580</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C25">
-        <v>82.550003051757798</v>
+        <v>113</v>
       </c>
       <c r="D25">
-        <v>84.5</v>
+        <v>114.449996948242</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>115.949996948242</v>
       </c>
       <c r="F25">
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>560</v>
+        <v>600</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C26">
-        <v>92.5</v>
+        <v>132.69999694824199</v>
       </c>
       <c r="D26">
-        <v>94.800003051757798</v>
+        <v>134.55000305175801</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -2420,52 +2617,6 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>580</v>
-      </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27">
-        <v>113</v>
-      </c>
-      <c r="D27">
-        <v>114.449996948242</v>
-      </c>
-      <c r="E27">
-        <v>115.949996948242</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>600</v>
-      </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28">
-        <v>132.69999694824199</v>
-      </c>
-      <c r="D28">
-        <v>134.55000305175801</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
         <v>0</v>
       </c>
     </row>
@@ -2476,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF63FBE-2A48-4693-BAFE-17FB0026C370}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2493,365 +2644,427 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="1">
         <v>45888</v>
       </c>
+      <c r="B2">
+        <v>416.09</v>
+      </c>
+      <c r="C2">
+        <v>415.79</v>
+      </c>
+      <c r="D2">
+        <v>3543629</v>
+      </c>
+      <c r="E2">
+        <v>23.2654</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45947</v>
+      <c r="A3" s="1">
+        <v>45889</v>
+      </c>
+      <c r="B3">
+        <v>420.59</v>
+      </c>
+      <c r="C3">
+        <v>420.46</v>
+      </c>
+      <c r="D3">
+        <v>4060195</v>
+      </c>
+      <c r="E3">
+        <v>23.230899999999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
+      <c r="A4" s="1">
+        <v>45890</v>
+      </c>
+      <c r="B4">
+        <v>417.89</v>
+      </c>
+      <c r="C4">
+        <v>417.68</v>
+      </c>
+      <c r="D4">
+        <v>2504344</v>
+      </c>
+      <c r="E4">
+        <v>24.808199999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
+      <c r="A5" s="1">
+        <v>45891</v>
+      </c>
+      <c r="B5">
+        <v>435.67</v>
+      </c>
+      <c r="C5">
+        <v>435.47</v>
+      </c>
+      <c r="D5">
+        <v>3785096</v>
+      </c>
+      <c r="E5">
+        <v>24.036899999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>45894</v>
+      </c>
+      <c r="B6">
+        <v>432.3</v>
+      </c>
+      <c r="C6">
+        <v>432.17</v>
+      </c>
+      <c r="D6">
+        <v>1858079</v>
+      </c>
+      <c r="E6">
+        <v>22.229600000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" t="s">
-        <v>74</v>
+      <c r="A7" s="1">
+        <v>45895</v>
+      </c>
+      <c r="B7">
+        <v>431.26</v>
+      </c>
+      <c r="C7">
+        <v>431.35</v>
+      </c>
+      <c r="D7">
+        <v>2792215</v>
+      </c>
+      <c r="E7">
+        <v>23.700399999999998</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>45947</v>
+        <v>45896</v>
       </c>
       <c r="B8">
-        <v>527.08000000000004</v>
+        <v>432.67</v>
       </c>
       <c r="C8">
-        <v>527.07000000000005</v>
+        <v>432.81</v>
       </c>
       <c r="D8">
-        <v>2814681</v>
+        <v>1971269</v>
       </c>
       <c r="E8">
-        <v>34.354999999999997</v>
+        <v>23.117799999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>45946</v>
+        <v>45897</v>
       </c>
       <c r="B9">
-        <v>540.96</v>
+        <v>434.91</v>
       </c>
       <c r="C9">
-        <v>541</v>
+        <v>435.08</v>
       </c>
       <c r="D9">
-        <v>3463082</v>
+        <v>1651718</v>
       </c>
       <c r="E9">
-        <v>35.454999999999998</v>
+        <v>22.2027</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>45945</v>
+        <v>45898</v>
       </c>
       <c r="B10">
-        <v>534.04999999999995</v>
+        <v>419.04</v>
       </c>
       <c r="C10">
-        <v>533.95000000000005</v>
+        <v>418.97</v>
       </c>
       <c r="D10">
-        <v>3447104</v>
+        <v>3673787</v>
       </c>
       <c r="E10">
-        <v>35.574399999999997</v>
+        <v>22.826699999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>45944</v>
+        <v>45902</v>
       </c>
       <c r="B11">
-        <v>527.47</v>
+        <v>416.05</v>
       </c>
       <c r="C11">
-        <v>527.54999999999995</v>
+        <v>415.85</v>
       </c>
       <c r="D11">
-        <v>5459830</v>
+        <v>2329944</v>
       </c>
       <c r="E11">
-        <v>29.365600000000001</v>
+        <v>23.8691</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>45943</v>
+        <v>45903</v>
       </c>
       <c r="B12">
-        <v>504.76</v>
+        <v>415.12</v>
       </c>
       <c r="C12">
-        <v>504.8</v>
+        <v>414.94</v>
       </c>
       <c r="D12">
-        <v>2618593</v>
+        <v>1496741</v>
       </c>
       <c r="E12">
-        <v>29.409300000000002</v>
+        <v>24.699200000000001</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>45940</v>
+        <v>45904</v>
       </c>
       <c r="B13">
-        <v>491.3</v>
+        <v>420.22</v>
       </c>
       <c r="C13">
-        <v>491.31</v>
+        <v>420.34</v>
       </c>
       <c r="D13">
-        <v>3889116</v>
+        <v>1634609</v>
       </c>
       <c r="E13">
-        <v>35.252699999999997</v>
+        <v>23.353400000000001</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>45939</v>
+        <v>45905</v>
       </c>
       <c r="B14">
-        <v>500.36</v>
+        <v>423.08</v>
       </c>
       <c r="C14">
-        <v>500.47</v>
+        <v>423.21</v>
       </c>
       <c r="D14">
-        <v>3114119</v>
+        <v>1843342</v>
       </c>
       <c r="E14">
-        <v>26.8504</v>
+        <v>23.042400000000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>45938</v>
+        <v>45908</v>
       </c>
       <c r="B15">
-        <v>502.12</v>
+        <v>422.78</v>
       </c>
       <c r="C15">
-        <v>502.09</v>
+        <v>422.94</v>
       </c>
       <c r="D15">
-        <v>3959416</v>
+        <v>1876960</v>
       </c>
       <c r="E15">
-        <v>28.336099999999998</v>
+        <v>23.001100000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>45937</v>
+        <v>45909</v>
       </c>
       <c r="B16">
-        <v>486.71</v>
+        <v>418.09</v>
       </c>
       <c r="C16">
-        <v>486.71</v>
+        <v>417.91</v>
       </c>
       <c r="D16">
-        <v>2135728</v>
+        <v>1710703</v>
       </c>
       <c r="E16">
-        <v>28.570900000000002</v>
+        <v>23.260100000000001</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>45936</v>
+        <v>45910</v>
       </c>
       <c r="B17">
-        <v>495.38</v>
+        <v>422.91</v>
       </c>
       <c r="C17">
-        <v>495.32</v>
+        <v>422.91</v>
       </c>
       <c r="D17">
-        <v>2629156</v>
+        <v>2221280</v>
       </c>
       <c r="E17">
-        <v>27.279299999999999</v>
+        <v>24.9328</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>45933</v>
+        <v>45911</v>
       </c>
       <c r="B18">
-        <v>497.85</v>
+        <v>431.38</v>
       </c>
       <c r="C18">
-        <v>498.03</v>
+        <v>431.33</v>
       </c>
       <c r="D18">
-        <v>2996868</v>
+        <v>2738072</v>
       </c>
       <c r="E18">
-        <v>26.299399999999999</v>
+        <v>23.968399999999999</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>45932</v>
+        <v>45912</v>
       </c>
       <c r="B19">
-        <v>490.57</v>
+        <v>431.52</v>
       </c>
       <c r="C19">
-        <v>490.95</v>
+        <v>431.28</v>
       </c>
       <c r="D19">
-        <v>2648753</v>
+        <v>2341766</v>
       </c>
       <c r="E19">
-        <v>24.940200000000001</v>
+        <v>23.8918</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>45931</v>
+        <v>45915</v>
       </c>
       <c r="B20">
-        <v>480.82</v>
+        <v>435.94</v>
       </c>
       <c r="C20">
-        <v>480.82</v>
+        <v>435.65</v>
       </c>
       <c r="D20">
-        <v>2964858</v>
+        <v>2255875</v>
       </c>
       <c r="E20">
-        <v>24.610399999999998</v>
+        <v>24.618300000000001</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>45930</v>
+        <v>45916</v>
       </c>
       <c r="B21">
-        <v>477.15</v>
+        <v>440.67</v>
       </c>
       <c r="C21">
-        <v>476.84</v>
+        <v>440.55</v>
       </c>
       <c r="D21">
-        <v>2315264</v>
+        <v>2366493</v>
       </c>
       <c r="E21">
-        <v>23.5016</v>
+        <v>26.8583</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>45929</v>
+        <v>45917</v>
       </c>
       <c r="B22">
-        <v>471.61</v>
+        <v>450.66</v>
       </c>
       <c r="C22">
-        <v>471.62</v>
+        <v>450.52</v>
       </c>
       <c r="D22">
-        <v>2892237</v>
+        <v>4512193</v>
       </c>
       <c r="E22">
-        <v>23.569800000000001</v>
+        <v>23.169499999999999</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>45926</v>
+        <v>45918</v>
       </c>
       <c r="B23">
-        <v>465.76</v>
+        <v>466.96</v>
       </c>
       <c r="C23">
-        <v>465.83</v>
+        <v>467.22</v>
       </c>
       <c r="D23">
-        <v>2329149</v>
+        <v>4331863</v>
       </c>
       <c r="E23">
-        <v>25.084299999999999</v>
+        <v>25.007100000000001</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>45925</v>
+        <v>45919</v>
       </c>
       <c r="B24">
-        <v>463.72</v>
+        <v>466.54</v>
       </c>
       <c r="C24">
-        <v>463.68</v>
+        <v>466.83</v>
       </c>
       <c r="D24">
-        <v>2979229</v>
+        <v>5069345</v>
       </c>
       <c r="E24">
-        <v>25.611599999999999</v>
+        <v>23.502700000000001</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>45924</v>
+        <v>45922</v>
       </c>
       <c r="B25">
-        <v>469.79</v>
+        <v>472.1</v>
       </c>
       <c r="C25">
-        <v>469.74</v>
+        <v>471.96</v>
       </c>
       <c r="D25">
-        <v>2776892</v>
+        <v>3179951</v>
       </c>
       <c r="E25">
-        <v>24.491399999999999</v>
+        <v>25.349699999999999</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -2873,817 +3086,592 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>45922</v>
+        <v>45924</v>
       </c>
       <c r="B27">
-        <v>472.1</v>
+        <v>469.79</v>
       </c>
       <c r="C27">
-        <v>471.96</v>
+        <v>469.74</v>
       </c>
       <c r="D27">
-        <v>3179951</v>
+        <v>2776892</v>
       </c>
       <c r="E27">
-        <v>25.349699999999999</v>
+        <v>24.491399999999999</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>45919</v>
+        <v>45925</v>
       </c>
       <c r="B28">
-        <v>466.54</v>
+        <v>463.72</v>
       </c>
       <c r="C28">
-        <v>466.83</v>
+        <v>463.68</v>
       </c>
       <c r="D28">
-        <v>5069345</v>
+        <v>2979229</v>
       </c>
       <c r="E28">
-        <v>23.502700000000001</v>
+        <v>25.611599999999999</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>45918</v>
+        <v>45926</v>
       </c>
       <c r="B29">
-        <v>466.96</v>
+        <v>465.76</v>
       </c>
       <c r="C29">
-        <v>467.22</v>
+        <v>465.83</v>
       </c>
       <c r="D29">
-        <v>4331863</v>
+        <v>2329149</v>
       </c>
       <c r="E29">
-        <v>25.007100000000001</v>
+        <v>25.084299999999999</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>45917</v>
+        <v>45929</v>
       </c>
       <c r="B30">
-        <v>450.66</v>
+        <v>471.61</v>
       </c>
       <c r="C30">
-        <v>450.52</v>
+        <v>471.62</v>
       </c>
       <c r="D30">
-        <v>4512193</v>
+        <v>2892237</v>
       </c>
       <c r="E30">
-        <v>23.169499999999999</v>
+        <v>23.569800000000001</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>45916</v>
+        <v>45930</v>
       </c>
       <c r="B31">
-        <v>440.67</v>
+        <v>477.15</v>
       </c>
       <c r="C31">
-        <v>440.55</v>
+        <v>476.84</v>
       </c>
       <c r="D31">
-        <v>2366493</v>
+        <v>2315264</v>
       </c>
       <c r="E31">
-        <v>26.8583</v>
+        <v>23.5016</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>45915</v>
+        <v>45931</v>
       </c>
       <c r="B32">
-        <v>435.94</v>
+        <v>480.82</v>
       </c>
       <c r="C32">
-        <v>435.65</v>
+        <v>480.82</v>
       </c>
       <c r="D32">
-        <v>2255875</v>
+        <v>2964858</v>
       </c>
       <c r="E32">
-        <v>24.618300000000001</v>
+        <v>24.610399999999998</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>45912</v>
+        <v>45932</v>
       </c>
       <c r="B33">
-        <v>431.52</v>
+        <v>490.57</v>
       </c>
       <c r="C33">
-        <v>431.28</v>
+        <v>490.95</v>
       </c>
       <c r="D33">
-        <v>2341766</v>
+        <v>2648753</v>
       </c>
       <c r="E33">
-        <v>23.8918</v>
+        <v>24.940200000000001</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>45911</v>
+        <v>45933</v>
       </c>
       <c r="B34">
-        <v>431.38</v>
+        <v>497.85</v>
       </c>
       <c r="C34">
-        <v>431.33</v>
+        <v>498.03</v>
       </c>
       <c r="D34">
-        <v>2738072</v>
+        <v>2996868</v>
       </c>
       <c r="E34">
-        <v>23.968399999999999</v>
+        <v>26.299399999999999</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>45910</v>
+        <v>45936</v>
       </c>
       <c r="B35">
-        <v>422.91</v>
+        <v>495.38</v>
       </c>
       <c r="C35">
-        <v>422.91</v>
+        <v>495.32</v>
       </c>
       <c r="D35">
-        <v>2221280</v>
+        <v>2629156</v>
       </c>
       <c r="E35">
-        <v>24.9328</v>
+        <v>27.279299999999999</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>45909</v>
+        <v>45937</v>
       </c>
       <c r="B36">
-        <v>418.09</v>
+        <v>486.71</v>
       </c>
       <c r="C36">
-        <v>417.91</v>
+        <v>486.71</v>
       </c>
       <c r="D36">
-        <v>1710703</v>
+        <v>2135728</v>
       </c>
       <c r="E36">
-        <v>23.260100000000001</v>
+        <v>28.570900000000002</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>45908</v>
+        <v>45938</v>
       </c>
       <c r="B37">
-        <v>422.78</v>
+        <v>502.12</v>
       </c>
       <c r="C37">
-        <v>422.94</v>
+        <v>502.09</v>
       </c>
       <c r="D37">
-        <v>1876960</v>
+        <v>3959416</v>
       </c>
       <c r="E37">
-        <v>23.001100000000001</v>
+        <v>28.336099999999998</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>45905</v>
+        <v>45939</v>
       </c>
       <c r="B38">
-        <v>423.08</v>
+        <v>500.36</v>
       </c>
       <c r="C38">
-        <v>423.21</v>
+        <v>500.47</v>
       </c>
       <c r="D38">
-        <v>1843342</v>
+        <v>3114119</v>
       </c>
       <c r="E38">
-        <v>23.042400000000001</v>
+        <v>26.8504</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>45904</v>
+        <v>45940</v>
       </c>
       <c r="B39">
-        <v>420.22</v>
+        <v>491.3</v>
       </c>
       <c r="C39">
-        <v>420.34</v>
+        <v>491.31</v>
       </c>
       <c r="D39">
-        <v>1634609</v>
+        <v>3889116</v>
       </c>
       <c r="E39">
-        <v>23.353400000000001</v>
+        <v>35.252699999999997</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>45903</v>
+        <v>45943</v>
       </c>
       <c r="B40">
-        <v>415.12</v>
+        <v>504.76</v>
       </c>
       <c r="C40">
-        <v>414.94</v>
+        <v>504.8</v>
       </c>
       <c r="D40">
-        <v>1496741</v>
+        <v>2618593</v>
       </c>
       <c r="E40">
-        <v>24.699200000000001</v>
+        <v>29.409300000000002</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>45902</v>
+        <v>45944</v>
       </c>
       <c r="B41">
-        <v>416.05</v>
+        <v>527.47</v>
       </c>
       <c r="C41">
-        <v>415.85</v>
+        <v>527.54999999999995</v>
       </c>
       <c r="D41">
-        <v>2329944</v>
+        <v>5459830</v>
       </c>
       <c r="E41">
-        <v>23.8691</v>
+        <v>29.365600000000001</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>45898</v>
+        <v>45945</v>
       </c>
       <c r="B42">
-        <v>419.04</v>
+        <v>534.04999999999995</v>
       </c>
       <c r="C42">
-        <v>418.97</v>
+        <v>533.95000000000005</v>
       </c>
       <c r="D42">
-        <v>3673787</v>
+        <v>3447104</v>
       </c>
       <c r="E42">
-        <v>22.826699999999999</v>
+        <v>35.574399999999997</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>45897</v>
+        <v>45946</v>
       </c>
       <c r="B43">
-        <v>434.91</v>
+        <v>540.96</v>
       </c>
       <c r="C43">
-        <v>435.08</v>
+        <v>541</v>
       </c>
       <c r="D43">
-        <v>1651718</v>
+        <v>3463082</v>
       </c>
       <c r="E43">
-        <v>22.2027</v>
+        <v>35.454999999999998</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>45896</v>
+        <v>45947</v>
       </c>
       <c r="B44">
-        <v>432.67</v>
+        <v>527.08000000000004</v>
       </c>
       <c r="C44">
-        <v>432.81</v>
+        <v>527.07000000000005</v>
       </c>
       <c r="D44">
-        <v>1971269</v>
+        <v>2814681</v>
       </c>
       <c r="E44">
-        <v>23.117799999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="1">
-        <v>45895</v>
-      </c>
-      <c r="B45">
-        <v>431.26</v>
-      </c>
-      <c r="C45">
-        <v>431.35</v>
-      </c>
-      <c r="D45">
-        <v>2792215</v>
-      </c>
-      <c r="E45">
-        <v>23.700399999999998</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="1">
-        <v>45894</v>
-      </c>
-      <c r="B46">
-        <v>432.3</v>
-      </c>
-      <c r="C46">
-        <v>432.17</v>
-      </c>
-      <c r="D46">
-        <v>1858079</v>
-      </c>
-      <c r="E46">
-        <v>22.229600000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
-        <v>45891</v>
-      </c>
-      <c r="B47">
-        <v>435.67</v>
-      </c>
-      <c r="C47">
-        <v>435.47</v>
-      </c>
-      <c r="D47">
-        <v>3785096</v>
-      </c>
-      <c r="E47">
-        <v>24.036899999999999</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
-        <v>45890</v>
-      </c>
-      <c r="B48">
-        <v>417.89</v>
-      </c>
-      <c r="C48">
-        <v>417.68</v>
-      </c>
-      <c r="D48">
-        <v>2504344</v>
-      </c>
-      <c r="E48">
-        <v>24.808199999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="1">
-        <v>45889</v>
-      </c>
-      <c r="B49">
-        <v>420.59</v>
-      </c>
-      <c r="C49">
-        <v>420.46</v>
-      </c>
-      <c r="D49">
-        <v>4060195</v>
-      </c>
-      <c r="E49">
-        <v>23.230899999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="1">
-        <v>45888</v>
-      </c>
-      <c r="B50">
-        <v>416.09</v>
-      </c>
-      <c r="C50">
-        <v>415.79</v>
-      </c>
-      <c r="D50">
-        <v>3543629</v>
-      </c>
-      <c r="E50">
-        <v>23.2654</v>
+        <v>34.354999999999997</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E44">
+    <sortCondition ref="A2:A44"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E334F64-B724-4BD5-8186-621E827CCBFF}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
         <v>45919</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="B2">
+        <v>4.0304E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>45922</v>
+      </c>
+      <c r="B3">
+        <v>4.0758999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>45923</v>
+      </c>
+      <c r="B4">
+        <v>4.0601000000000005E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>45924</v>
+      </c>
+      <c r="B5">
+        <v>4.0750000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>45925</v>
+      </c>
+      <c r="B6">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>45926</v>
+      </c>
+      <c r="B7">
+        <v>4.1069000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>45929</v>
+      </c>
+      <c r="B8">
+        <v>4.1269E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B9">
+        <v>4.1009000000000004E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45931</v>
+      </c>
+      <c r="B10">
+        <v>4.0750000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>45932</v>
+      </c>
+      <c r="B11">
+        <v>4.0948999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>45933</v>
+      </c>
+      <c r="B12">
+        <v>4.0738000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>45936</v>
+      </c>
+      <c r="B13">
+        <v>4.1116E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>45937</v>
+      </c>
+      <c r="B14">
+        <v>4.0906999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>45938</v>
+      </c>
+      <c r="B15">
+        <v>4.0800999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>45939</v>
+      </c>
+      <c r="B16">
+        <v>4.0795999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>45940</v>
+      </c>
+      <c r="B17">
+        <v>4.0738000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B18">
+        <v>4.0738000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>45944</v>
+      </c>
+      <c r="B19">
+        <v>4.0631E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B20">
+        <v>4.0856000000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>45946</v>
+      </c>
+      <c r="B21">
+        <v>4.0774999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>45947</v>
+      </c>
+      <c r="B22">
+        <v>4.0431999999999996E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>45950</v>
+      </c>
+      <c r="B23">
+        <v>4.0350999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>45951</v>
+      </c>
+      <c r="B24">
+        <v>4.0091000000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B25">
+        <v>4.0060999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>45953</v>
+      </c>
+      <c r="B26">
+        <v>4.0057000000000002E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>45954</v>
+      </c>
+      <c r="B27">
+        <v>3.9844999999999998E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>45957</v>
+      </c>
+      <c r="B28">
+        <v>4.0018999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>45958</v>
+      </c>
+      <c r="B29">
+        <v>3.9580999999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B30">
+        <v>3.9296000000000005E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>45960</v>
+      </c>
+      <c r="B31">
+        <v>3.9266999999999996E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
         <v>45961</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>45961</v>
-      </c>
-      <c r="B7">
-        <v>3.8978000000000002</v>
-      </c>
-      <c r="C7">
-        <v>-0.73640000000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>45960</v>
-      </c>
-      <c r="B8">
-        <v>3.9266999999999999</v>
-      </c>
-      <c r="C8">
-        <v>-7.5600000000000001E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
-        <v>45959</v>
-      </c>
-      <c r="B9">
-        <v>3.9296000000000002</v>
-      </c>
-      <c r="C9">
-        <v>-0.71919999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>45958</v>
-      </c>
-      <c r="B10">
-        <v>3.9581</v>
-      </c>
-      <c r="C10">
-        <v>-1.0941000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
-        <v>45957</v>
-      </c>
-      <c r="B11">
-        <v>4.0019</v>
-      </c>
-      <c r="C11">
-        <v>0.43709999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
-        <v>45954</v>
-      </c>
-      <c r="B12">
-        <v>3.9845000000000002</v>
-      </c>
-      <c r="C12">
-        <v>-0.5292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
-        <v>45953</v>
-      </c>
-      <c r="B13">
-        <v>4.0057</v>
-      </c>
-      <c r="C13">
-        <v>-1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
-        <v>45952</v>
-      </c>
-      <c r="B14">
-        <v>4.0061</v>
-      </c>
-      <c r="C14">
-        <v>-7.46E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
-        <v>45951</v>
-      </c>
-      <c r="B15">
-        <v>4.0091000000000001</v>
-      </c>
-      <c r="C15">
-        <v>-0.64300000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>45950</v>
-      </c>
-      <c r="B16">
-        <v>4.0350999999999999</v>
-      </c>
-      <c r="C16">
-        <v>-0.20030000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>45947</v>
-      </c>
-      <c r="B17">
-        <v>4.0431999999999997</v>
-      </c>
-      <c r="C17">
-        <v>-0.84240000000000004</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <v>45946</v>
-      </c>
-      <c r="B18">
-        <v>4.0774999999999997</v>
-      </c>
-      <c r="C18">
-        <v>-0.19839999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>45945</v>
-      </c>
-      <c r="B19">
-        <v>4.0856000000000003</v>
-      </c>
-      <c r="C19">
-        <v>0.55369999999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <v>45944</v>
-      </c>
-      <c r="B20">
-        <v>4.0631000000000004</v>
-      </c>
-      <c r="C20">
-        <v>-0.2616</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <v>45943</v>
-      </c>
-      <c r="B21">
-        <v>4.0738000000000003</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>45940</v>
-      </c>
-      <c r="B22">
-        <v>4.0738000000000003</v>
-      </c>
-      <c r="C22">
-        <v>-0.1429</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>45939</v>
-      </c>
-      <c r="B23">
-        <v>4.0796000000000001</v>
-      </c>
-      <c r="C23">
-        <v>-1.12E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>45938</v>
-      </c>
-      <c r="B24">
-        <v>4.0800999999999998</v>
-      </c>
-      <c r="C24">
-        <v>-0.26050000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>45937</v>
-      </c>
-      <c r="B25">
-        <v>4.0907</v>
-      </c>
-      <c r="C25">
-        <v>-0.50749999999999995</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
-        <v>45936</v>
-      </c>
-      <c r="B26">
-        <v>4.1116000000000001</v>
-      </c>
-      <c r="C26">
-        <v>0.92800000000000005</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <v>45933</v>
-      </c>
-      <c r="B27">
-        <v>4.0738000000000003</v>
-      </c>
-      <c r="C27">
-        <v>-0.51580000000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="1">
-        <v>45932</v>
-      </c>
-      <c r="B28">
-        <v>4.0949</v>
-      </c>
-      <c r="C28">
-        <v>0.48920000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
-        <v>45931</v>
-      </c>
-      <c r="B29">
-        <v>4.0750000000000002</v>
-      </c>
-      <c r="C29">
-        <v>-0.63290000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="1">
-        <v>45930</v>
-      </c>
-      <c r="B30">
-        <v>4.1009000000000002</v>
-      </c>
-      <c r="C30">
-        <v>-0.62919999999999998</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="1">
-        <v>45929</v>
-      </c>
-      <c r="B31">
-        <v>4.1269</v>
-      </c>
-      <c r="C31">
-        <v>0.48559999999999998</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>45926</v>
-      </c>
       <c r="B32">
-        <v>4.1069000000000004</v>
-      </c>
-      <c r="C32">
-        <v>0.1694</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>45925</v>
-      </c>
-      <c r="B33">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C33">
-        <v>0.61429999999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>45924</v>
-      </c>
-      <c r="B34">
-        <v>4.0750000000000002</v>
-      </c>
-      <c r="C34">
-        <v>0.36570000000000003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>45923</v>
-      </c>
-      <c r="B35">
-        <v>4.0601000000000003</v>
-      </c>
-      <c r="C35">
-        <v>-0.3866</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
-        <v>45922</v>
-      </c>
-      <c r="B36">
-        <v>4.0758999999999999</v>
-      </c>
-      <c r="C36">
-        <v>1.1279999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
-        <v>45919</v>
-      </c>
-      <c r="B37">
-        <v>4.0304000000000002</v>
-      </c>
-      <c r="C37">
-        <v>-1.1442000000000001</v>
+        <v>3.8977999999999999E-2</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3692,8 +3680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CBEB46-6427-4BE9-80D8-2E7838DFCB46}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3703,7 +3691,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -3711,7 +3699,7 @@
         <v>530</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>2.9999997466802601E-2</v>
@@ -3727,6 +3715,155 @@
       </c>
       <c r="G7">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5C50C5-7014-4B1C-9522-5D24AF9F336A}">
+  <dimension ref="A1:O39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean CAT data, need daily time series of ATM call
</commit_message>
<xml_diff>
--- a/data/raw/CAT_Options_Data.xlsx
+++ b/data/raw/CAT_Options_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/david_crowe_ucdconnect_ie/Documents/Masters/FIN42020 - Derivative Securities/Project/FIN42020-Derivative-Securities-Project/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{1FD50B2D-D1A4-41A4-ADFD-D06D56F95791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A28B259D-590E-4D92-BFA9-C85FCC48993F}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{1FD50B2D-D1A4-41A4-ADFD-D06D56F95791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{296F64FE-A2AE-4498-B44D-BD0D0FE27096}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Price" sheetId="3" r:id="rId3"/>
     <sheet name="USGG1M" sheetId="4" r:id="rId4"/>
     <sheet name="ATM" sheetId="5" r:id="rId5"/>
-    <sheet name="Metadata" sheetId="7" r:id="rId6"/>
+    <sheet name="MetaData" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t>Strike</t>
   </si>
@@ -229,11 +229,30 @@
     <t>Rate</t>
   </si>
   <si>
+    <t>“Closing prices for all options (all of the strikes available for puts and calls) on your assigned trade date of 19th September 2025 with an expiry date of 17th October 2025.”</t>
+  </si>
+  <si>
+    <t>“Closing prices for the At The Money (ATM) call option (strike as close as possible to closing price of stock) on your trade date.”</t>
+  </si>
+  <si>
+    <t>“Prices for that same option strike for each date from 19th September 2025 to 17th October 2025 inclusive (required to delta hedge the option).”</t>
+  </si>
+  <si>
+    <t>“Closing prices for your stock for matching dates and a history of prices leading up to the trade date to estimate historical volatility.”</t>
+  </si>
+  <si>
+    <t>1. Full option chain on the trade date</t>
+  </si>
+  <si>
+    <t>2.  ATM call price on the trade date</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">This is a standard </t>
+      <t xml:space="preserve">3. Daily prices for that </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <i/>
         <sz val="11"/>
         <color theme="1"/>
@@ -241,17 +260,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>option chain</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for </t>
+      <t>same</t>
     </r>
     <r>
       <rPr>
@@ -262,54 +271,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>one single date</t>
+      <t xml:space="preserve"> ATM call from 19 Sep to 17 Oct</t>
     </r>
+  </si>
+  <si>
+    <t>4. Stock prices for matching dates + history before trade date</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (17 October 2025).</t>
-    </r>
-  </si>
-  <si>
-    <t>The same</t>
-  </si>
-  <si>
-    <t>This is the only problem.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">It has </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>one row</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from the option chain:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This is </t>
+      <t xml:space="preserve">Trade-date underlying = </t>
     </r>
     <r>
       <rPr>
@@ -320,7 +290,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>not</t>
+      <t>466.54</t>
     </r>
     <r>
       <rPr>
@@ -330,110 +300,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> an ATM time series.</t>
+      <t xml:space="preserve"> on 19 Sep 2025.</t>
     </r>
   </si>
   <si>
-    <t>It is just one observation for one date.</t>
-  </si>
-  <si>
-    <t>From the bottom of the Price sheet:</t>
-  </si>
-  <si>
-    <t>Trade date = 2025-08-19</t>
-  </si>
-  <si>
-    <t>Underlying price (PX_LAST) = 416.09</t>
-  </si>
-  <si>
-    <t>This is the day you enter the option position for the delta hedge.</t>
-  </si>
-  <si>
-    <t>This is the ONLY correct date to determine the ATM strike.</t>
-  </si>
-  <si>
-    <t>Correct ATM strike selection</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Trade-date underlying price = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>416.09</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Closest strike to 416.09 is 420.</t>
-  </si>
-  <si>
-    <t>So the ATM strike is:</t>
-  </si>
-  <si>
-    <t>CAT 10/17/25 C420 (or P420, but call is standard)</t>
-  </si>
-  <si>
-    <t>This is your ATM option.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">You need the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>daily price</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> of: CAT 10/17/25 C420 2025-08-19 → 2025-10-17</t>
-    </r>
-  </si>
-  <si>
-    <t>1. Calls Sheets</t>
-  </si>
-  <si>
-    <t>2. Puts Sheet</t>
-  </si>
-  <si>
-    <t>3. Price Sheet</t>
-  </si>
-  <si>
-    <t>4. USGG1M sheet</t>
-  </si>
-  <si>
-    <t>This is the stock price history.</t>
-  </si>
-  <si>
-    <t>Rate data</t>
-  </si>
-  <si>
-    <t>5. ATM sheet</t>
-  </si>
-  <si>
-    <t>For the delta hedging simulation, the project requires:“Daily prices of the same ATM option from the trade date up to expiration.”</t>
+    <t>Daily closing prices of CAT 10/17/25 C470 from 19 Sep 2025 to 17 Oct 2025 inclusive.</t>
   </si>
 </sst>
 </file>
@@ -582,6 +453,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -932,11 +804,17 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1900,94 +1778,94 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2630,7 +2508,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3678,10 +3556,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31CBEB46-6427-4BE9-80D8-2E7838DFCB46}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3689,32 +3567,19 @@
     <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>530</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7">
-        <v>2.9999997466802601E-2</v>
-      </c>
-      <c r="D7">
-        <v>1.4899997711181601</v>
-      </c>
-      <c r="E7">
-        <v>0.60000002384185802</v>
-      </c>
-      <c r="F7">
-        <v>26.7674045562744</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3723,147 +3588,65 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5C50C5-7014-4B1C-9522-5D24AF9F336A}">
-  <dimension ref="A1:O39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC50146-0074-49CD-9749-E676CAF1B329}">
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>82</v>
+      <c r="A1" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>86</v>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>87</v>
+      <c r="A11" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A15" s="4" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add historical volatility notebook and update IV analysis
</commit_message>
<xml_diff>
--- a/data/raw/CAT_Options_Data.xlsx
+++ b/data/raw/CAT_Options_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/david_crowe_ucdconnect_ie/Documents/Masters/FIN42020 - Derivative Securities/Project/FIN42020-Derivative-Securities-Project/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{1FD50B2D-D1A4-41A4-ADFD-D06D56F95791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8DDAC24-B0C7-458B-AE41-926A13C85B42}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{1FD50B2D-D1A4-41A4-ADFD-D06D56F95791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C5BC5C3-6B3F-482F-B552-45DCC351A78A}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-16365" windowWidth="29130" windowHeight="15810" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calls" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
   <si>
     <t>Strike</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>“Closing prices for all options (all of the strikes available for puts and calls) on your assigned trade date of 19th September 2025 with an expiry date of 17th October 2025.”</t>
@@ -322,7 +319,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -821,14 +818,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1792,94 +1789,94 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
+      <c r="A63" s="6"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3"/>
+      <c r="A81" s="6"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3570,31 +3567,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1A609E-5604-4BBA-8844-472105F0EABB}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
       <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>45887</v>
       </c>
       <c r="B2">
@@ -3605,7 +3602,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>45888</v>
       </c>
       <c r="B3">
@@ -3616,7 +3613,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>45889</v>
       </c>
       <c r="B4">
@@ -3627,7 +3624,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>45890</v>
       </c>
       <c r="B5">
@@ -3638,7 +3635,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>45891</v>
       </c>
       <c r="B6">
@@ -3649,7 +3646,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>45894</v>
       </c>
       <c r="B7">
@@ -3660,7 +3657,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>45895</v>
       </c>
       <c r="B8">
@@ -3671,7 +3668,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>45896</v>
       </c>
       <c r="B9">
@@ -3682,7 +3679,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>45897</v>
       </c>
       <c r="B10">
@@ -3693,7 +3690,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>45898</v>
       </c>
       <c r="B11">
@@ -3704,387 +3701,376 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
-        <v>45901</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" t="s">
-        <v>63</v>
+      <c r="A12" s="5">
+        <v>45902</v>
+      </c>
+      <c r="B12">
+        <v>1.27</v>
+      </c>
+      <c r="C12">
+        <v>1.26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
-        <v>45902</v>
+      <c r="A13" s="5">
+        <v>45903</v>
       </c>
       <c r="B13">
-        <v>1.27</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1.26</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
-        <v>45903</v>
+      <c r="A14" s="5">
+        <v>45904</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="C14">
-        <v>0.93</v>
+        <v>1.23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
-        <v>45904</v>
+      <c r="A15" s="5">
+        <v>45905</v>
       </c>
       <c r="B15">
-        <v>1.3</v>
+        <v>1.43</v>
       </c>
       <c r="C15">
-        <v>1.23</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
-        <v>45905</v>
+      <c r="A16" s="5">
+        <v>45908</v>
       </c>
       <c r="B16">
-        <v>1.43</v>
+        <v>1.21</v>
       </c>
       <c r="C16">
-        <v>1.34</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
-        <v>45908</v>
+      <c r="A17" s="5">
+        <v>45909</v>
       </c>
       <c r="B17">
-        <v>1.21</v>
+        <v>0.91</v>
       </c>
       <c r="C17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="5">
+        <v>45910</v>
+      </c>
+      <c r="B18">
+        <v>1.5</v>
+      </c>
+      <c r="C18">
         <v>1.18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
-        <v>45909</v>
-      </c>
-      <c r="B18">
-        <v>0.91</v>
-      </c>
-      <c r="C18">
-        <v>0.3</v>
-      </c>
-    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
-        <v>45910</v>
+      <c r="A19" s="5">
+        <v>45911</v>
       </c>
       <c r="B19">
-        <v>1.5</v>
+        <v>2.35</v>
       </c>
       <c r="C19">
-        <v>1.18</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
-        <v>45911</v>
+      <c r="A20" s="5">
+        <v>45912</v>
       </c>
       <c r="B20">
-        <v>2.35</v>
+        <v>1.95</v>
       </c>
       <c r="C20">
-        <v>2.13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
-        <v>45912</v>
+      <c r="A21" s="5">
+        <v>45915</v>
       </c>
       <c r="B21">
-        <v>1.95</v>
+        <v>2.73</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
-        <v>45915</v>
+      <c r="A22" s="5">
+        <v>45916</v>
       </c>
       <c r="B22">
-        <v>2.73</v>
+        <v>3.55</v>
       </c>
       <c r="C22">
-        <v>2.6</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
-        <v>45916</v>
+      <c r="A23" s="5">
+        <v>45917</v>
       </c>
       <c r="B23">
-        <v>3.55</v>
+        <v>6.06</v>
       </c>
       <c r="C23">
-        <v>3.5</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
-        <v>45917</v>
+      <c r="A24" s="5">
+        <v>45918</v>
       </c>
       <c r="B24">
-        <v>6.06</v>
+        <v>13.46</v>
       </c>
       <c r="C24">
-        <v>5.6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
-        <v>45918</v>
+      <c r="A25" s="5">
+        <v>45919</v>
       </c>
       <c r="B25">
-        <v>13.46</v>
+        <v>12.1</v>
       </c>
       <c r="C25">
-        <v>13</v>
+        <v>12.05</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
-        <v>45919</v>
+      <c r="A26" s="5">
+        <v>45922</v>
       </c>
       <c r="B26">
-        <v>12.1</v>
+        <v>14.73</v>
       </c>
       <c r="C26">
-        <v>12.05</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
-        <v>45922</v>
+      <c r="A27" s="5">
+        <v>45923</v>
       </c>
       <c r="B27">
-        <v>14.73</v>
+        <v>15.01</v>
       </c>
       <c r="C27">
-        <v>14.4</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
-        <v>45923</v>
+      <c r="A28" s="5">
+        <v>45924</v>
       </c>
       <c r="B28">
-        <v>15.01</v>
+        <v>12.77</v>
       </c>
       <c r="C28">
-        <v>13.9</v>
+        <v>12.45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
-        <v>45924</v>
+      <c r="A29" s="5">
+        <v>45925</v>
       </c>
       <c r="B29">
-        <v>12.77</v>
+        <v>9.5</v>
       </c>
       <c r="C29">
-        <v>12.45</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
-        <v>45925</v>
+      <c r="A30" s="5">
+        <v>45926</v>
       </c>
       <c r="B30">
-        <v>9.5</v>
+        <v>8.74</v>
       </c>
       <c r="C30">
-        <v>9.25</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
-        <v>45926</v>
+      <c r="A31" s="5">
+        <v>45929</v>
       </c>
       <c r="B31">
-        <v>8.74</v>
+        <v>11.92</v>
       </c>
       <c r="C31">
-        <v>9.4</v>
+        <v>11.55</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
-        <v>45929</v>
+      <c r="A32" s="5">
+        <v>45930</v>
       </c>
       <c r="B32">
-        <v>11.92</v>
+        <v>14.65</v>
       </c>
       <c r="C32">
-        <v>11.55</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="6">
-        <v>45930</v>
+      <c r="A33" s="5">
+        <v>45931</v>
       </c>
       <c r="B33">
-        <v>14.65</v>
+        <v>16.86</v>
       </c>
       <c r="C33">
-        <v>14.55</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
-        <v>45931</v>
+      <c r="A34" s="5">
+        <v>45932</v>
       </c>
       <c r="B34">
-        <v>16.86</v>
+        <v>25</v>
       </c>
       <c r="C34">
-        <v>17.2</v>
+        <v>24.35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
-        <v>45932</v>
+      <c r="A35" s="5">
+        <v>45933</v>
       </c>
       <c r="B35">
-        <v>25</v>
+        <v>32.85</v>
       </c>
       <c r="C35">
-        <v>24.35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="6">
-        <v>45933</v>
+      <c r="A36" s="5">
+        <v>45936</v>
       </c>
       <c r="B36">
-        <v>32.85</v>
+        <v>29.01</v>
       </c>
       <c r="C36">
-        <v>30</v>
+        <v>27.55</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="6">
-        <v>45936</v>
+      <c r="A37" s="5">
+        <v>45937</v>
       </c>
       <c r="B37">
-        <v>29.01</v>
+        <v>20.2</v>
       </c>
       <c r="C37">
-        <v>27.55</v>
+        <v>20.45</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
-        <v>45937</v>
+      <c r="A38" s="5">
+        <v>45938</v>
       </c>
       <c r="B38">
-        <v>20.2</v>
+        <v>34.340000000000003</v>
       </c>
       <c r="C38">
-        <v>20.45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="6">
-        <v>45938</v>
+      <c r="A39" s="5">
+        <v>45939</v>
       </c>
       <c r="B39">
-        <v>34.340000000000003</v>
+        <v>33.28</v>
       </c>
       <c r="C39">
-        <v>33</v>
+        <v>31.15</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="6">
-        <v>45939</v>
+      <c r="A40" s="5">
+        <v>45940</v>
       </c>
       <c r="B40">
-        <v>33.28</v>
+        <v>29.13</v>
       </c>
       <c r="C40">
-        <v>31.15</v>
+        <v>23.7</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
-        <v>45940</v>
+      <c r="A41" s="5">
+        <v>45943</v>
       </c>
       <c r="B41">
-        <v>29.13</v>
+        <v>35.39</v>
       </c>
       <c r="C41">
-        <v>23.7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="6">
-        <v>45943</v>
+      <c r="A42" s="5">
+        <v>45944</v>
       </c>
       <c r="B42">
-        <v>35.39</v>
+        <v>59.67</v>
       </c>
       <c r="C42">
-        <v>35</v>
+        <v>56.85</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="6">
-        <v>45944</v>
+      <c r="A43" s="5">
+        <v>45945</v>
       </c>
       <c r="B43">
-        <v>59.67</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="C43">
-        <v>56.85</v>
+        <v>62.85</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="6">
-        <v>45945</v>
+      <c r="A44" s="5">
+        <v>45946</v>
       </c>
       <c r="B44">
-        <v>64.900000000000006</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="C44">
-        <v>62.85</v>
+        <v>70.75</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="6">
-        <v>45946</v>
+      <c r="A45" s="5">
+        <v>45947</v>
       </c>
       <c r="B45">
-        <v>70.099999999999994</v>
+        <v>60.15</v>
       </c>
       <c r="C45">
-        <v>70.75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="6">
-        <v>45947</v>
-      </c>
-      <c r="B46">
-        <v>60.15</v>
-      </c>
-      <c r="C46">
         <v>56.15</v>
       </c>
     </row>
@@ -4097,25 +4083,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0046F26-DC89-4643-8F24-A505D593A526}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -4135,54 +4121,54 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>64</v>
+      <c r="A3" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>65</v>
+      <c r="A7" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>66</v>
+      <c r="A11" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>67</v>
+      <c r="A15" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 02 call vs put smile plot
</commit_message>
<xml_diff>
--- a/data/raw/CAT_Options_Data.xlsx
+++ b/data/raw/CAT_Options_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/david_crowe_ucdconnect_ie/Documents/Masters/FIN42020 - Derivative Securities/Project/FIN42020-Derivative-Securities-Project/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{1FD50B2D-D1A4-41A4-ADFD-D06D56F95791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C5BC5C3-6B3F-482F-B552-45DCC351A78A}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{1FD50B2D-D1A4-41A4-ADFD-D06D56F95791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD25EB83-FCDF-4BCA-A9DC-AD56A188DF9E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calls" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Price" sheetId="3" r:id="rId3"/>
     <sheet name="USGG1M" sheetId="4" r:id="rId4"/>
     <sheet name="ATM" sheetId="9" r:id="rId5"/>
-    <sheet name="ATM Option" sheetId="10" r:id="rId6"/>
-    <sheet name="MetaData" sheetId="8" r:id="rId7"/>
+    <sheet name="Dividends" sheetId="11" r:id="rId6"/>
+    <sheet name="ATM Option" sheetId="10" r:id="rId7"/>
+    <sheet name="MetaData" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
   <si>
     <t>Strike</t>
   </si>
@@ -312,6 +313,69 @@
   </si>
   <si>
     <t>Bid Price</t>
+  </si>
+  <si>
+    <t>Declaration</t>
+  </si>
+  <si>
+    <t>Ex Date</t>
+  </si>
+  <si>
+    <t>Record</t>
+  </si>
+  <si>
+    <t>Payable</t>
+  </si>
+  <si>
+    <t>Curr</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>BDVD Projection</t>
+  </si>
+  <si>
+    <t>Regular Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We obtained the CAT dividend schedule from Bloomberg. </t>
+  </si>
+  <si>
+    <t>The ex dates around our trade date (19 Sep 2025) are:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 21 Jul 2025 (already passed), and </t>
+  </si>
+  <si>
+    <t>- 20 Oct 2025 (after the option expiry 17 Oct 2025).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hence there are no cash dividends paid between the trade date and the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">option maturity. For the life of this option the stock behaves as a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">non dividend paying asset, so the standard Black Scholes and put–call </t>
+  </si>
+  <si>
+    <t xml:space="preserve">parity formulas without dividends are appropriate. We therefore set </t>
+  </si>
+  <si>
+    <t>the dividend yield $q = 0$.</t>
+  </si>
+  <si>
+    <t>Dividend assumption</t>
   </si>
 </sst>
 </file>
@@ -814,7 +878,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -825,6 +889,8 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="43">
@@ -3569,7 +3635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1A609E-5604-4BBA-8844-472105F0EABB}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -4080,6 +4146,327 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CB94FF-4EB1-413A-BD1D-CBF62EB12DA8}">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
+    <col min="5" max="5" width="4.453125" customWidth="1"/>
+    <col min="6" max="6" width="7.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>46001</v>
+      </c>
+      <c r="B2" s="1">
+        <v>46042</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45950</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45981</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>45936</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45950</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45950</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45981</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>45819</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45859</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45859</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45889</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1.51</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>45756</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45768</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45768</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45797</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1.41</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>45636</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45678</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45678</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45708</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1.41</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>45574</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45586</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45586</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45616</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1.41</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>45455</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45495</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45495</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45524</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1.41</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>45392</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45401</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45404</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45432</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>45273</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45310</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45313</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45342</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0046F26-DC89-4643-8F24-A505D593A526}">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -4109,7 +4496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC50146-0074-49CD-9749-E676CAF1B329}">
   <dimension ref="A1:A15"/>
   <sheetViews>

</xml_diff>